<commit_message>
Update Open-Boiler.xlsx, ~$Open-Boiler.xlsx, and 2 more files...
</commit_message>
<xml_diff>
--- a/software/sw-tests/tst-01/extra/Heat-Levels.xlsx
+++ b/software/sw-tests/tst-01/extra/Heat-Levels.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gcasanova\source\Repos\GitHub\open-boiler\software\sw-tests\tst-01\extra\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\casanovg\source\Repos\GitHub\open-boiler\software\sw-tests\tst-01\extra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F4C7116-9978-4803-A268-38DFA7AB2024}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D9AAEED-E394-423F-ABD0-52A966A310F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="6" xr2:uid="{0E7AC8B7-8509-410A-BE79-7988297E2B94}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="6" xr2:uid="{0E7AC8B7-8509-410A-BE79-7988297E2B94}"/>
   </bookViews>
   <sheets>
     <sheet name="Analysis-A" sheetId="2" r:id="rId1"/>
@@ -35,6 +35,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1066,8 +1067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A24BA88-A765-4701-917B-81E571016397}">
   <dimension ref="B2:BN1340"/>
   <sheetViews>
-    <sheetView topLeftCell="AH486" workbookViewId="0">
-      <selection sqref="A1:AO502"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1260,15 +1261,14 @@
         <v>343</v>
       </c>
       <c r="K4" s="52">
-        <f>COUNTIFS(F:F,"&gt;=" &amp; J6, F:F,"&lt;=" &amp; K6, E:E,"&gt;0.998", E:E, "&lt;1.002")</f>
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="L4" s="2">
         <v>1023</v>
       </c>
       <c r="M4" s="2">
         <f>ROUND(L4/K4,0)</f>
-        <v>21</v>
+        <v>1023</v>
       </c>
       <c r="O4" s="2">
         <f>0</f>
@@ -1276,107 +1276,107 @@
       </c>
       <c r="P4" s="47">
         <f>IF(O4+($M$4)&lt;=$L$4,O4+($M$4),$L$4)</f>
-        <v>21</v>
+        <v>1023</v>
       </c>
       <c r="Q4" s="47">
         <f>IF(P4+($M$4)&lt;=$L$4,P4+($M$4),$L$4)</f>
-        <v>42</v>
+        <v>1023</v>
       </c>
       <c r="R4" s="47">
         <f t="shared" ref="R4:AN4" si="0">IF(Q4+($M$4)&lt;=$L$4,Q4+($M$4),$L$4)</f>
-        <v>63</v>
+        <v>1023</v>
       </c>
       <c r="S4" s="47">
         <f t="shared" si="0"/>
-        <v>84</v>
+        <v>1023</v>
       </c>
       <c r="T4" s="47">
         <f t="shared" si="0"/>
-        <v>105</v>
+        <v>1023</v>
       </c>
       <c r="U4" s="47">
         <f t="shared" si="0"/>
-        <v>126</v>
+        <v>1023</v>
       </c>
       <c r="V4" s="47">
         <f t="shared" si="0"/>
-        <v>147</v>
+        <v>1023</v>
       </c>
       <c r="W4" s="47">
         <f t="shared" si="0"/>
-        <v>168</v>
+        <v>1023</v>
       </c>
       <c r="X4" s="47">
         <f t="shared" si="0"/>
-        <v>189</v>
+        <v>1023</v>
       </c>
       <c r="Y4" s="47">
         <f t="shared" si="0"/>
-        <v>210</v>
+        <v>1023</v>
       </c>
       <c r="Z4" s="47">
         <f t="shared" si="0"/>
-        <v>231</v>
+        <v>1023</v>
       </c>
       <c r="AA4" s="47">
         <f t="shared" si="0"/>
-        <v>252</v>
+        <v>1023</v>
       </c>
       <c r="AB4" s="47">
         <f t="shared" si="0"/>
-        <v>273</v>
+        <v>1023</v>
       </c>
       <c r="AC4" s="47">
         <f t="shared" si="0"/>
-        <v>294</v>
+        <v>1023</v>
       </c>
       <c r="AD4" s="47">
         <f t="shared" si="0"/>
-        <v>315</v>
+        <v>1023</v>
       </c>
       <c r="AE4" s="47">
         <f t="shared" si="0"/>
-        <v>336</v>
+        <v>1023</v>
       </c>
       <c r="AF4" s="47">
         <f t="shared" si="0"/>
-        <v>357</v>
+        <v>1023</v>
       </c>
       <c r="AG4" s="47">
         <f t="shared" si="0"/>
-        <v>378</v>
+        <v>1023</v>
       </c>
       <c r="AH4" s="47">
         <f t="shared" si="0"/>
-        <v>399</v>
+        <v>1023</v>
       </c>
       <c r="AI4" s="47">
         <f t="shared" si="0"/>
-        <v>420</v>
+        <v>1023</v>
       </c>
       <c r="AJ4" s="47">
         <f t="shared" si="0"/>
-        <v>441</v>
+        <v>1023</v>
       </c>
       <c r="AK4" s="47">
         <f t="shared" si="0"/>
-        <v>462</v>
+        <v>1023</v>
       </c>
       <c r="AL4" s="47">
         <f t="shared" si="0"/>
-        <v>483</v>
+        <v>1023</v>
       </c>
       <c r="AM4" s="47">
         <f t="shared" si="0"/>
-        <v>504</v>
+        <v>1023</v>
       </c>
       <c r="AN4" s="47">
         <f t="shared" si="0"/>
-        <v>525</v>
+        <v>1023</v>
       </c>
       <c r="AO4" s="47">
         <f>IF(AN4+($M$4)&lt;=$L$4,AN4+($M$4),$L$4)</f>
-        <v>546</v>
+        <v>1023</v>
       </c>
       <c r="AP4" s="47"/>
       <c r="AQ4" s="47"/>
@@ -1428,111 +1428,111 @@
       <c r="M5" s="2"/>
       <c r="O5" s="47">
         <f>IF(O4+($M$4-1)&lt;=$L$4, O4+($M$4-1), $L$4)</f>
-        <v>20</v>
+        <v>1022</v>
       </c>
       <c r="P5" s="47">
         <f t="shared" ref="P5:AO5" si="1">IF(P4+($M$4-1)&lt;=$L$4, P4+($M$4-1), $L$4)</f>
-        <v>41</v>
+        <v>1023</v>
       </c>
       <c r="Q5" s="47">
         <f t="shared" si="1"/>
-        <v>62</v>
+        <v>1023</v>
       </c>
       <c r="R5" s="47">
         <f t="shared" ref="R5" si="2">IF(R4+($M$4-1)&lt;=$L$4, R4+($M$4-1), $L$4)</f>
-        <v>83</v>
+        <v>1023</v>
       </c>
       <c r="S5" s="47">
         <f t="shared" ref="S5" si="3">IF(S4+($M$4-1)&lt;=$L$4, S4+($M$4-1), $L$4)</f>
-        <v>104</v>
+        <v>1023</v>
       </c>
       <c r="T5" s="47">
         <f t="shared" ref="T5" si="4">IF(T4+($M$4-1)&lt;=$L$4, T4+($M$4-1), $L$4)</f>
-        <v>125</v>
+        <v>1023</v>
       </c>
       <c r="U5" s="47">
         <f t="shared" ref="U5" si="5">IF(U4+($M$4-1)&lt;=$L$4, U4+($M$4-1), $L$4)</f>
-        <v>146</v>
+        <v>1023</v>
       </c>
       <c r="V5" s="47">
         <f t="shared" ref="V5" si="6">IF(V4+($M$4-1)&lt;=$L$4, V4+($M$4-1), $L$4)</f>
-        <v>167</v>
+        <v>1023</v>
       </c>
       <c r="W5" s="47">
         <f t="shared" ref="W5" si="7">IF(W4+($M$4-1)&lt;=$L$4, W4+($M$4-1), $L$4)</f>
-        <v>188</v>
+        <v>1023</v>
       </c>
       <c r="X5" s="47">
         <f t="shared" ref="X5" si="8">IF(X4+($M$4-1)&lt;=$L$4, X4+($M$4-1), $L$4)</f>
-        <v>209</v>
+        <v>1023</v>
       </c>
       <c r="Y5" s="47">
         <f t="shared" ref="Y5" si="9">IF(Y4+($M$4-1)&lt;=$L$4, Y4+($M$4-1), $L$4)</f>
-        <v>230</v>
+        <v>1023</v>
       </c>
       <c r="Z5" s="47">
         <f t="shared" ref="Z5" si="10">IF(Z4+($M$4-1)&lt;=$L$4, Z4+($M$4-1), $L$4)</f>
-        <v>251</v>
+        <v>1023</v>
       </c>
       <c r="AA5" s="47">
         <f t="shared" ref="AA5" si="11">IF(AA4+($M$4-1)&lt;=$L$4, AA4+($M$4-1), $L$4)</f>
-        <v>272</v>
+        <v>1023</v>
       </c>
       <c r="AB5" s="47">
         <f t="shared" ref="AB5" si="12">IF(AB4+($M$4-1)&lt;=$L$4, AB4+($M$4-1), $L$4)</f>
-        <v>293</v>
+        <v>1023</v>
       </c>
       <c r="AC5" s="47">
         <f t="shared" ref="AC5" si="13">IF(AC4+($M$4-1)&lt;=$L$4, AC4+($M$4-1), $L$4)</f>
-        <v>314</v>
+        <v>1023</v>
       </c>
       <c r="AD5" s="47">
         <f t="shared" ref="AD5" si="14">IF(AD4+($M$4-1)&lt;=$L$4, AD4+($M$4-1), $L$4)</f>
-        <v>335</v>
+        <v>1023</v>
       </c>
       <c r="AE5" s="47">
         <f t="shared" ref="AE5" si="15">IF(AE4+($M$4-1)&lt;=$L$4, AE4+($M$4-1), $L$4)</f>
-        <v>356</v>
+        <v>1023</v>
       </c>
       <c r="AF5" s="47">
         <f t="shared" ref="AF5" si="16">IF(AF4+($M$4-1)&lt;=$L$4, AF4+($M$4-1), $L$4)</f>
-        <v>377</v>
+        <v>1023</v>
       </c>
       <c r="AG5" s="47">
         <f t="shared" ref="AG5" si="17">IF(AG4+($M$4-1)&lt;=$L$4, AG4+($M$4-1), $L$4)</f>
-        <v>398</v>
+        <v>1023</v>
       </c>
       <c r="AH5" s="47">
         <f t="shared" ref="AH5" si="18">IF(AH4+($M$4-1)&lt;=$L$4, AH4+($M$4-1), $L$4)</f>
-        <v>419</v>
+        <v>1023</v>
       </c>
       <c r="AI5" s="47">
         <f t="shared" ref="AI5" si="19">IF(AI4+($M$4-1)&lt;=$L$4, AI4+($M$4-1), $L$4)</f>
-        <v>440</v>
+        <v>1023</v>
       </c>
       <c r="AJ5" s="47">
         <f t="shared" ref="AJ5" si="20">IF(AJ4+($M$4-1)&lt;=$L$4, AJ4+($M$4-1), $L$4)</f>
-        <v>461</v>
+        <v>1023</v>
       </c>
       <c r="AK5" s="47">
         <f t="shared" ref="AK5" si="21">IF(AK4+($M$4-1)&lt;=$L$4, AK4+($M$4-1), $L$4)</f>
-        <v>482</v>
+        <v>1023</v>
       </c>
       <c r="AL5" s="47">
         <f t="shared" ref="AL5" si="22">IF(AL4+($M$4-1)&lt;=$L$4, AL4+($M$4-1), $L$4)</f>
-        <v>503</v>
+        <v>1023</v>
       </c>
       <c r="AM5" s="47">
         <f t="shared" ref="AM5" si="23">IF(AM4+($M$4-1)&lt;=$L$4, AM4+($M$4-1), $L$4)</f>
-        <v>524</v>
+        <v>1023</v>
       </c>
       <c r="AN5" s="47">
         <f t="shared" ref="AN5" si="24">IF(AN4+($M$4-1)&lt;=$L$4, AN4+($M$4-1), $L$4)</f>
-        <v>545</v>
+        <v>1023</v>
       </c>
       <c r="AO5" s="47">
         <f t="shared" si="1"/>
-        <v>566</v>
+        <v>1023</v>
       </c>
       <c r="AP5" s="47"/>
       <c r="AQ5" s="47"/>
@@ -52163,18 +52163,22 @@
         <v>343</v>
       </c>
       <c r="K4" s="52">
-        <f>COUNTIFS(F:F,"&gt;=" &amp; J6, F:F,"&lt;=" &amp; K6, E:E,"&gt;0.998", E:E, "&lt;1.002")</f>
+        <f>COUNTIFS(F:F,"&gt;=" &amp; J6, F:F,"&lt;=" &amp; K6, E:E,"&gt;99,8%", E:E, "&lt;100,02%")</f>
         <v>12</v>
       </c>
       <c r="L4" s="2">
         <v>1023</v>
       </c>
       <c r="M4" s="2">
-        <f>ROUND(L4/K4,0)</f>
+        <f>ROUND(L4/(K4),0)</f>
         <v>85</v>
       </c>
+      <c r="N4" s="2">
+        <f t="shared" ref="N4:O4" si="0">ROUND(M4/(L4+1),0)</f>
+        <v>0</v>
+      </c>
       <c r="O4" s="2">
-        <f>0</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P4" s="47">
@@ -52186,95 +52190,95 @@
         <v>170</v>
       </c>
       <c r="R4" s="47">
-        <f t="shared" ref="R4:AN4" si="0">IF(Q4+($M$4)&lt;=$L$4,Q4+($M$4),$L$4)</f>
+        <f t="shared" ref="R4:AN4" si="1">IF(Q4+($M$4)&lt;=$L$4,Q4+($M$4),$L$4)</f>
         <v>255</v>
       </c>
       <c r="S4" s="47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>340</v>
       </c>
       <c r="T4" s="47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>425</v>
       </c>
       <c r="U4" s="47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>510</v>
       </c>
       <c r="V4" s="47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>595</v>
       </c>
       <c r="W4" s="47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>680</v>
       </c>
       <c r="X4" s="47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>765</v>
       </c>
       <c r="Y4" s="47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>850</v>
       </c>
       <c r="Z4" s="47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>935</v>
       </c>
       <c r="AA4" s="47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1020</v>
       </c>
       <c r="AB4" s="47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1023</v>
       </c>
       <c r="AC4" s="47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1023</v>
       </c>
       <c r="AD4" s="47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1023</v>
       </c>
       <c r="AE4" s="47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1023</v>
       </c>
       <c r="AF4" s="47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1023</v>
       </c>
       <c r="AG4" s="47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1023</v>
       </c>
       <c r="AH4" s="47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1023</v>
       </c>
       <c r="AI4" s="47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1023</v>
       </c>
       <c r="AJ4" s="47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1023</v>
       </c>
       <c r="AK4" s="47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1023</v>
       </c>
       <c r="AL4" s="47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1023</v>
       </c>
       <c r="AM4" s="47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1023</v>
       </c>
       <c r="AN4" s="47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1023</v>
       </c>
       <c r="AO4" s="47">
@@ -52309,107 +52313,107 @@
         <v>84</v>
       </c>
       <c r="P5" s="47">
-        <f t="shared" ref="P5:AO5" si="1">IF(P4+($M$4-1)&lt;=$L$4, P4+($M$4-1), $L$4)</f>
+        <f t="shared" ref="P5:AO5" si="2">IF(P4+($M$4-1)&lt;=$L$4, P4+($M$4-1), $L$4)</f>
         <v>169</v>
       </c>
       <c r="Q5" s="47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>254</v>
       </c>
       <c r="R5" s="47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>339</v>
       </c>
       <c r="S5" s="47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>424</v>
       </c>
       <c r="T5" s="47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>509</v>
       </c>
       <c r="U5" s="47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>594</v>
       </c>
       <c r="V5" s="47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>679</v>
       </c>
       <c r="W5" s="47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>764</v>
       </c>
       <c r="X5" s="47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>849</v>
       </c>
       <c r="Y5" s="47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>934</v>
       </c>
       <c r="Z5" s="47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1019</v>
       </c>
       <c r="AA5" s="47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1023</v>
       </c>
       <c r="AB5" s="47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1023</v>
       </c>
       <c r="AC5" s="47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1023</v>
       </c>
       <c r="AD5" s="47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1023</v>
       </c>
       <c r="AE5" s="47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1023</v>
       </c>
       <c r="AF5" s="47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1023</v>
       </c>
       <c r="AG5" s="47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1023</v>
       </c>
       <c r="AH5" s="47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1023</v>
       </c>
       <c r="AI5" s="47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1023</v>
       </c>
       <c r="AJ5" s="47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1023</v>
       </c>
       <c r="AK5" s="47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1023</v>
       </c>
       <c r="AL5" s="47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1023</v>
       </c>
       <c r="AM5" s="47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1023</v>
       </c>
       <c r="AN5" s="47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1023</v>
       </c>
       <c r="AO5" s="47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1023</v>
       </c>
     </row>
@@ -52436,30 +52440,102 @@
       </c>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
-      <c r="S6" s="2"/>
-      <c r="T6" s="2"/>
-      <c r="U6" s="2"/>
-      <c r="V6" s="2"/>
-      <c r="W6" s="2"/>
-      <c r="X6" s="2"/>
-      <c r="Y6" s="2"/>
-      <c r="Z6" s="2"/>
-      <c r="AA6" s="2"/>
-      <c r="AB6" s="2"/>
-      <c r="AC6" s="2"/>
-      <c r="AD6" s="2"/>
-      <c r="AE6" s="2"/>
-      <c r="AF6" s="2"/>
-      <c r="AG6" s="2"/>
-      <c r="AH6" s="2"/>
-      <c r="AI6" s="2"/>
-      <c r="AJ6" s="2"/>
-      <c r="AK6" s="2"/>
-      <c r="AL6" s="2"/>
+      <c r="O6" s="47">
+        <f>$L$4-O5</f>
+        <v>939</v>
+      </c>
+      <c r="P6" s="47">
+        <f t="shared" ref="P6:AL6" si="3">$L$4-P5</f>
+        <v>854</v>
+      </c>
+      <c r="Q6" s="47">
+        <f t="shared" si="3"/>
+        <v>769</v>
+      </c>
+      <c r="R6" s="47">
+        <f t="shared" si="3"/>
+        <v>684</v>
+      </c>
+      <c r="S6" s="47">
+        <f t="shared" si="3"/>
+        <v>599</v>
+      </c>
+      <c r="T6" s="47">
+        <f t="shared" si="3"/>
+        <v>514</v>
+      </c>
+      <c r="U6" s="47">
+        <f t="shared" si="3"/>
+        <v>429</v>
+      </c>
+      <c r="V6" s="47">
+        <f t="shared" si="3"/>
+        <v>344</v>
+      </c>
+      <c r="W6" s="47">
+        <f t="shared" si="3"/>
+        <v>259</v>
+      </c>
+      <c r="X6" s="47">
+        <f t="shared" si="3"/>
+        <v>174</v>
+      </c>
+      <c r="Y6" s="47">
+        <f t="shared" si="3"/>
+        <v>89</v>
+      </c>
+      <c r="Z6" s="47">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="AA6" s="47">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AB6" s="47">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AC6" s="47">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AD6" s="47">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AE6" s="47">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AF6" s="47">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AG6" s="47">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AH6" s="47">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AI6" s="47">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AJ6" s="47">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AK6" s="47">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AL6" s="47">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="AM6" s="2"/>
       <c r="AN6" s="2"/>
       <c r="AO6" s="2"/>
@@ -52507,6 +52583,10 @@
       <c r="Q8" s="59" t="s">
         <v>58</v>
       </c>
+      <c r="R8" s="59"/>
+      <c r="S8" s="59"/>
+      <c r="T8" s="59"/>
+      <c r="U8" s="59"/>
     </row>
     <row r="9" spans="2:41" x14ac:dyDescent="0.25">
       <c r="B9" s="54">
@@ -52528,7 +52608,7 @@
         <v>0.86999999999999988</v>
       </c>
       <c r="I9" s="58">
-        <f t="shared" ref="I9:I36" si="2">SUM(K9:M9)</f>
+        <f t="shared" ref="I9:I36" si="4">SUM(K9:M9)</f>
         <v>100</v>
       </c>
       <c r="J9" s="58">
@@ -52553,7 +52633,7 @@
       </c>
       <c r="Q9" t="str">
         <f>CONCATENATE("{{",K9, ", ", L9, ", ", M9, "}, ",ROUND(N9,0), ", ", ROUND(O9,3),"}, /* Heat level ", J9, " = ",ROUND(N9,0), " Kcal/h */")</f>
-        <v>{{100, 0, 0}, 7000, 0.87}, /* Heat level 0 = 7000 Kcal/h */</v>
+        <v>{{100, 0, 0}, 7000, 0,87}, /* Heat level 0 = 7000 Kcal/h */</v>
       </c>
     </row>
     <row r="10" spans="2:41" x14ac:dyDescent="0.25">
@@ -52576,7 +52656,7 @@
         <v>0.96833333333333327</v>
       </c>
       <c r="I10" s="58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="J10" s="58">
@@ -52592,16 +52672,16 @@
         <v>0</v>
       </c>
       <c r="N10" s="56">
-        <f t="shared" ref="N10:N36" si="3">F10</f>
+        <f t="shared" ref="N10:N36" si="5">F10</f>
         <v>7833.333333333333</v>
       </c>
       <c r="O10" s="11">
-        <f t="shared" ref="O10:O36" si="4">G10</f>
+        <f t="shared" ref="O10:O36" si="6">G10</f>
         <v>0.96833333333333327</v>
       </c>
       <c r="Q10" t="str">
-        <f t="shared" ref="Q10:Q36" si="5">CONCATENATE("{{",K10, ", ", L10, ", ", M10, "}, ",ROUND(N10,0), ", ", ROUND(O10,3),"}, /* Heat level ", J10, " = ",ROUND(N10,0), " Kcal/h */")</f>
-        <v>{{83, 17, 0}, 7833, 0.968}, /* Heat level 1 = 7833 Kcal/h */</v>
+        <f t="shared" ref="Q10:Q36" si="7">CONCATENATE("{{",K10, ", ", L10, ", ", M10, "}, ",ROUND(N10,0), ", ", ROUND(O10,3),"}, /* Heat level ", J10, " = ",ROUND(N10,0), " Kcal/h */")</f>
+        <v>{{83, 17, 0}, 7833, 0,968}, /* Heat level 1 = 7833 Kcal/h */</v>
       </c>
       <c r="S10" s="1"/>
     </row>
@@ -52625,7 +52705,7 @@
         <v>1.0666666666666667</v>
       </c>
       <c r="I11" s="58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="J11" s="58">
@@ -52641,16 +52721,16 @@
         <v>0</v>
       </c>
       <c r="N11" s="56">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>8666.6666666666661</v>
       </c>
       <c r="O11" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.0666666666666667</v>
       </c>
       <c r="Q11" t="str">
-        <f t="shared" si="5"/>
-        <v>{{67, 33, 0}, 8667, 1.067}, /* Heat level 2 = 8667 Kcal/h */</v>
+        <f t="shared" si="7"/>
+        <v>{{67, 33, 0}, 8667, 1,067}, /* Heat level 2 = 8667 Kcal/h */</v>
       </c>
       <c r="S11" s="1"/>
     </row>
@@ -52674,7 +52754,7 @@
         <v>1.1233333333333333</v>
       </c>
       <c r="I12" s="58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="J12" s="58">
@@ -52690,16 +52770,16 @@
         <v>17</v>
       </c>
       <c r="N12" s="56">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>9166.6666666666661</v>
       </c>
       <c r="O12" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.1233333333333333</v>
       </c>
       <c r="Q12" t="str">
-        <f t="shared" si="5"/>
-        <v>{{83, 0, 17}, 9167, 1.123}, /* Heat level 3 = 9167 Kcal/h */</v>
+        <f t="shared" si="7"/>
+        <v>{{83, 0, 17}, 9167, 1,123}, /* Heat level 3 = 9167 Kcal/h */</v>
       </c>
       <c r="S12" s="1"/>
     </row>
@@ -52723,7 +52803,7 @@
         <v>1.165</v>
       </c>
       <c r="I13" s="58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="J13" s="58">
@@ -52739,16 +52819,16 @@
         <v>0</v>
       </c>
       <c r="N13" s="56">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>9500</v>
       </c>
       <c r="O13" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.165</v>
       </c>
       <c r="Q13" t="str">
-        <f t="shared" si="5"/>
-        <v>{{50, 50, 0}, 9500, 1.165}, /* Heat level 4 = 9500 Kcal/h */</v>
+        <f t="shared" si="7"/>
+        <v>{{50, 50, 0}, 9500, 1,165}, /* Heat level 4 = 9500 Kcal/h */</v>
       </c>
       <c r="S13" s="1"/>
     </row>
@@ -52772,7 +52852,7 @@
         <v>1.2216666666666667</v>
       </c>
       <c r="I14" s="58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="J14" s="58">
@@ -52788,16 +52868,16 @@
         <v>16</v>
       </c>
       <c r="N14" s="56">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>10000</v>
       </c>
       <c r="O14" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.2216666666666667</v>
       </c>
       <c r="Q14" t="str">
-        <f t="shared" si="5"/>
-        <v>{{67, 17, 16}, 10000, 1.222}, /* Heat level 5 = 10000 Kcal/h */</v>
+        <f t="shared" si="7"/>
+        <v>{{67, 17, 16}, 10000, 1,222}, /* Heat level 5 = 10000 Kcal/h */</v>
       </c>
       <c r="S14" s="1"/>
     </row>
@@ -52821,7 +52901,7 @@
         <v>1.2633333333333332</v>
       </c>
       <c r="I15" s="58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="J15" s="58">
@@ -52837,16 +52917,16 @@
         <v>0</v>
       </c>
       <c r="N15" s="56">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>10333.333333333332</v>
       </c>
       <c r="O15" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.2633333333333332</v>
       </c>
       <c r="Q15" t="str">
-        <f t="shared" si="5"/>
-        <v>{{33, 67, 0}, 10333, 1.263}, /* Heat level 6 = 10333 Kcal/h */</v>
+        <f t="shared" si="7"/>
+        <v>{{33, 67, 0}, 10333, 1,263}, /* Heat level 6 = 10333 Kcal/h */</v>
       </c>
       <c r="S15" s="1"/>
     </row>
@@ -52870,7 +52950,7 @@
         <v>1.3199999999999998</v>
       </c>
       <c r="I16" s="58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="J16" s="58">
@@ -52886,16 +52966,16 @@
         <v>17</v>
       </c>
       <c r="N16" s="56">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>10833.333333333332</v>
       </c>
       <c r="O16" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.3199999999999998</v>
       </c>
       <c r="Q16" t="str">
-        <f t="shared" si="5"/>
-        <v>{{50, 33, 17}, 10833, 1.32}, /* Heat level 7 = 10833 Kcal/h */</v>
+        <f t="shared" si="7"/>
+        <v>{{50, 33, 17}, 10833, 1,32}, /* Heat level 7 = 10833 Kcal/h */</v>
       </c>
       <c r="S16" s="1"/>
     </row>
@@ -52919,7 +52999,7 @@
         <v>1.3616666666666666</v>
       </c>
       <c r="I17" s="58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="J17" s="58">
@@ -52935,16 +53015,16 @@
         <v>0</v>
       </c>
       <c r="N17" s="56">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>11166.666666666666</v>
       </c>
       <c r="O17" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.3616666666666666</v>
       </c>
       <c r="Q17" t="str">
-        <f t="shared" si="5"/>
-        <v>{{17, 83, 0}, 11167, 1.362}, /* Heat level 8 = 11167 Kcal/h */</v>
+        <f t="shared" si="7"/>
+        <v>{{17, 83, 0}, 11167, 1,362}, /* Heat level 8 = 11167 Kcal/h */</v>
       </c>
       <c r="S17" s="1"/>
     </row>
@@ -52968,7 +53048,7 @@
         <v>1.3766666666666665</v>
       </c>
       <c r="I18" s="58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="J18" s="58">
@@ -52984,16 +53064,16 @@
         <v>33</v>
       </c>
       <c r="N18" s="56">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>11333.333333333332</v>
       </c>
       <c r="O18" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.3766666666666665</v>
       </c>
       <c r="Q18" t="str">
-        <f t="shared" si="5"/>
-        <v>{{67, 0, 33}, 11333, 1.377}, /* Heat level 9 = 11333 Kcal/h */</v>
+        <f t="shared" si="7"/>
+        <v>{{67, 0, 33}, 11333, 1,377}, /* Heat level 9 = 11333 Kcal/h */</v>
       </c>
       <c r="S18" s="1"/>
     </row>
@@ -53017,7 +53097,7 @@
         <v>1.4183333333333334</v>
       </c>
       <c r="I19" s="58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="J19" s="58">
@@ -53033,16 +53113,16 @@
         <v>17</v>
       </c>
       <c r="N19" s="56">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>11666.666666666664</v>
       </c>
       <c r="O19" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.4183333333333334</v>
       </c>
       <c r="Q19" t="str">
-        <f t="shared" si="5"/>
-        <v>{{33, 50, 17}, 11667, 1.418}, /* Heat level 10 = 11667 Kcal/h */</v>
+        <f t="shared" si="7"/>
+        <v>{{33, 50, 17}, 11667, 1,418}, /* Heat level 10 = 11667 Kcal/h */</v>
       </c>
       <c r="S19" s="1"/>
     </row>
@@ -53066,7 +53146,7 @@
         <v>1.4599999999999997</v>
       </c>
       <c r="I20" s="58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="J20" s="58">
@@ -53082,16 +53162,16 @@
         <v>0</v>
       </c>
       <c r="N20" s="56">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>11999.999999999998</v>
       </c>
       <c r="O20" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.4599999999999997</v>
       </c>
       <c r="Q20" t="str">
-        <f t="shared" si="5"/>
-        <v>{{0, 100, 0}, 12000, 1.46}, /* Heat level 11 = 12000 Kcal/h */</v>
+        <f t="shared" si="7"/>
+        <v>{{0, 100, 0}, 12000, 1,46}, /* Heat level 11 = 12000 Kcal/h */</v>
       </c>
       <c r="S20" s="1"/>
     </row>
@@ -53115,7 +53195,7 @@
         <v>1.4750000000000001</v>
       </c>
       <c r="I21" s="58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="J21" s="58">
@@ -53131,16 +53211,16 @@
         <v>33</v>
       </c>
       <c r="N21" s="56">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>12166.666666666666</v>
       </c>
       <c r="O21" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.4750000000000001</v>
       </c>
       <c r="Q21" t="str">
-        <f t="shared" si="5"/>
-        <v>{{50, 17, 33}, 12167, 1.475}, /* Heat level 12 = 12167 Kcal/h */</v>
+        <f t="shared" si="7"/>
+        <v>{{50, 17, 33}, 12167, 1,475}, /* Heat level 12 = 12167 Kcal/h */</v>
       </c>
       <c r="S21" s="1"/>
     </row>
@@ -53164,7 +53244,7 @@
         <v>1.5166666666666666</v>
       </c>
       <c r="I22" s="58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="J22" s="58">
@@ -53180,16 +53260,16 @@
         <v>16</v>
       </c>
       <c r="N22" s="56">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>12500</v>
       </c>
       <c r="O22" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.5166666666666666</v>
       </c>
       <c r="Q22" t="str">
-        <f t="shared" si="5"/>
-        <v>{{17, 67, 16}, 12500, 1.517}, /* Heat level 13 = 12500 Kcal/h */</v>
+        <f t="shared" si="7"/>
+        <v>{{17, 67, 16}, 12500, 1,517}, /* Heat level 13 = 12500 Kcal/h */</v>
       </c>
       <c r="S22" s="1"/>
     </row>
@@ -53213,7 +53293,7 @@
         <v>1.5733333333333333</v>
       </c>
       <c r="I23" s="58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="J23" s="58">
@@ -53229,16 +53309,16 @@
         <v>33</v>
       </c>
       <c r="N23" s="56">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>13000</v>
       </c>
       <c r="O23" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.5733333333333333</v>
       </c>
       <c r="Q23" t="str">
-        <f t="shared" si="5"/>
-        <v>{{34, 33, 33}, 13000, 1.573}, /* Heat level 14 = 13000 Kcal/h */</v>
+        <f t="shared" si="7"/>
+        <v>{{34, 33, 33}, 13000, 1,573}, /* Heat level 14 = 13000 Kcal/h */</v>
       </c>
       <c r="S23" s="1"/>
     </row>
@@ -53262,7 +53342,7 @@
         <v>1.6149999999999998</v>
       </c>
       <c r="I24" s="58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="J24" s="58">
@@ -53278,16 +53358,16 @@
         <v>17</v>
       </c>
       <c r="N24" s="56">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>13333.333333333332</v>
       </c>
       <c r="O24" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.6149999999999998</v>
       </c>
       <c r="Q24" t="str">
-        <f t="shared" si="5"/>
-        <v>{{0, 83, 17}, 13333, 1.615}, /* Heat level 15 = 13333 Kcal/h */</v>
+        <f t="shared" si="7"/>
+        <v>{{0, 83, 17}, 13333, 1,615}, /* Heat level 15 = 13333 Kcal/h */</v>
       </c>
       <c r="S24" s="1"/>
     </row>
@@ -53311,7 +53391,7 @@
         <v>1.6300000000000001</v>
       </c>
       <c r="I25" s="58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="J25" s="58">
@@ -53327,16 +53407,16 @@
         <v>50</v>
       </c>
       <c r="N25" s="56">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>13500</v>
       </c>
       <c r="O25" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.6300000000000001</v>
       </c>
       <c r="Q25" t="str">
-        <f t="shared" si="5"/>
-        <v>{{50, 0, 50}, 13500, 1.63}, /* Heat level 16 = 13500 Kcal/h */</v>
+        <f t="shared" si="7"/>
+        <v>{{50, 0, 50}, 13500, 1,63}, /* Heat level 16 = 13500 Kcal/h */</v>
       </c>
       <c r="S25" s="1"/>
     </row>
@@ -53360,7 +53440,7 @@
         <v>1.6716666666666666</v>
       </c>
       <c r="I26" s="58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="J26" s="58">
@@ -53376,16 +53456,16 @@
         <v>33</v>
       </c>
       <c r="N26" s="56">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>13833.333333333332</v>
       </c>
       <c r="O26" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.6716666666666666</v>
       </c>
       <c r="Q26" t="str">
-        <f t="shared" si="5"/>
-        <v>{{17, 50, 33}, 13833, 1.672}, /* Heat level 17 = 13833 Kcal/h */</v>
+        <f t="shared" si="7"/>
+        <v>{{17, 50, 33}, 13833, 1,672}, /* Heat level 17 = 13833 Kcal/h */</v>
       </c>
       <c r="S26" s="1"/>
     </row>
@@ -53409,7 +53489,7 @@
         <v>1.7283333333333335</v>
       </c>
       <c r="I27" s="58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="J27" s="58">
@@ -53425,16 +53505,16 @@
         <v>50</v>
       </c>
       <c r="N27" s="56">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>14333.333333333332</v>
       </c>
       <c r="O27" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.7283333333333335</v>
       </c>
       <c r="Q27" t="str">
-        <f t="shared" si="5"/>
-        <v>{{33, 17, 50}, 14333, 1.728}, /* Heat level 18 = 14333 Kcal/h */</v>
+        <f t="shared" si="7"/>
+        <v>{{33, 17, 50}, 14333, 1,728}, /* Heat level 18 = 14333 Kcal/h */</v>
       </c>
       <c r="S27" s="1"/>
     </row>
@@ -53458,7 +53538,7 @@
         <v>1.77</v>
       </c>
       <c r="I28" s="58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="J28" s="58">
@@ -53474,16 +53554,16 @@
         <v>33</v>
       </c>
       <c r="N28" s="56">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>14666.666666666666</v>
       </c>
       <c r="O28" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.77</v>
       </c>
       <c r="Q28" t="str">
-        <f t="shared" si="5"/>
-        <v>{{0, 67, 33}, 14667, 1.77}, /* Heat level 19 = 14667 Kcal/h */</v>
+        <f t="shared" si="7"/>
+        <v>{{0, 67, 33}, 14667, 1,77}, /* Heat level 19 = 14667 Kcal/h */</v>
       </c>
       <c r="S28" s="1"/>
     </row>
@@ -53507,7 +53587,7 @@
         <v>1.8266666666666667</v>
       </c>
       <c r="I29" s="58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="J29" s="58">
@@ -53523,16 +53603,16 @@
         <v>50</v>
       </c>
       <c r="N29" s="56">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>15166.666666666666</v>
       </c>
       <c r="O29" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.8266666666666667</v>
       </c>
       <c r="Q29" t="str">
-        <f t="shared" si="5"/>
-        <v>{{17, 33, 50}, 15167, 1.827}, /* Heat level 20 = 15167 Kcal/h */</v>
+        <f t="shared" si="7"/>
+        <v>{{17, 33, 50}, 15167, 1,827}, /* Heat level 20 = 15167 Kcal/h */</v>
       </c>
       <c r="S29" s="1"/>
     </row>
@@ -53556,7 +53636,7 @@
         <v>1.8833333333333333</v>
       </c>
       <c r="I30" s="58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="J30" s="58">
@@ -53572,16 +53652,16 @@
         <v>67</v>
       </c>
       <c r="N30" s="56">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>15666.666666666664</v>
       </c>
       <c r="O30" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.8833333333333333</v>
       </c>
       <c r="Q30" t="str">
-        <f t="shared" si="5"/>
-        <v>{{33, 0, 67}, 15667, 1.883}, /* Heat level 21 = 15667 Kcal/h */</v>
+        <f t="shared" si="7"/>
+        <v>{{33, 0, 67}, 15667, 1,883}, /* Heat level 21 = 15667 Kcal/h */</v>
       </c>
       <c r="S30" s="1"/>
     </row>
@@ -53605,7 +53685,7 @@
         <v>1.925</v>
       </c>
       <c r="I31" s="58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="J31" s="58">
@@ -53621,16 +53701,16 @@
         <v>50</v>
       </c>
       <c r="N31" s="56">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>16000</v>
       </c>
       <c r="O31" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.925</v>
       </c>
       <c r="Q31" t="str">
-        <f t="shared" si="5"/>
-        <v>{{0, 50, 50}, 16000, 1.925}, /* Heat level 22 = 16000 Kcal/h */</v>
+        <f t="shared" si="7"/>
+        <v>{{0, 50, 50}, 16000, 1,925}, /* Heat level 22 = 16000 Kcal/h */</v>
       </c>
       <c r="S31" s="1"/>
     </row>
@@ -53654,7 +53734,7 @@
         <v>1.9816666666666665</v>
       </c>
       <c r="I32" s="58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="J32" s="58">
@@ -53670,16 +53750,16 @@
         <v>66</v>
       </c>
       <c r="N32" s="56">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>16500</v>
       </c>
       <c r="O32" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.9816666666666665</v>
       </c>
       <c r="Q32" t="str">
-        <f t="shared" si="5"/>
-        <v>{{17, 17, 66}, 16500, 1.982}, /* Heat level 23 = 16500 Kcal/h */</v>
+        <f t="shared" si="7"/>
+        <v>{{17, 17, 66}, 16500, 1,982}, /* Heat level 23 = 16500 Kcal/h */</v>
       </c>
       <c r="S32" s="1"/>
     </row>
@@ -53703,7 +53783,7 @@
         <v>2.08</v>
       </c>
       <c r="I33" s="58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="J33" s="58">
@@ -53719,16 +53799,16 @@
         <v>67</v>
       </c>
       <c r="N33" s="56">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>17333.333333333332</v>
       </c>
       <c r="O33" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2.08</v>
       </c>
       <c r="Q33" t="str">
-        <f t="shared" si="5"/>
-        <v>{{0, 33, 67}, 17333, 2.08}, /* Heat level 24 = 17333 Kcal/h */</v>
+        <f t="shared" si="7"/>
+        <v>{{0, 33, 67}, 17333, 2,08}, /* Heat level 24 = 17333 Kcal/h */</v>
       </c>
       <c r="S33" s="1"/>
     </row>
@@ -53752,7 +53832,7 @@
         <v>2.1366666666666667</v>
       </c>
       <c r="I34" s="58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="J34" s="58">
@@ -53768,16 +53848,16 @@
         <v>83</v>
       </c>
       <c r="N34" s="56">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>17833.333333333332</v>
       </c>
       <c r="O34" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2.1366666666666667</v>
       </c>
       <c r="Q34" t="str">
-        <f t="shared" si="5"/>
-        <v>{{17, 0, 83}, 17833, 2.137}, /* Heat level 25 = 17833 Kcal/h */</v>
+        <f t="shared" si="7"/>
+        <v>{{17, 0, 83}, 17833, 2,137}, /* Heat level 25 = 17833 Kcal/h */</v>
       </c>
       <c r="S34" s="1"/>
     </row>
@@ -53801,7 +53881,7 @@
         <v>2.2349999999999999</v>
       </c>
       <c r="I35" s="58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="J35" s="58">
@@ -53817,16 +53897,16 @@
         <v>83</v>
       </c>
       <c r="N35" s="56">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>18666.666666666664</v>
       </c>
       <c r="O35" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2.2349999999999999</v>
       </c>
       <c r="Q35" t="str">
-        <f t="shared" si="5"/>
-        <v>{{0, 17, 83}, 18667, 2.235}, /* Heat level 26 = 18667 Kcal/h */</v>
+        <f t="shared" si="7"/>
+        <v>{{0, 17, 83}, 18667, 2,235}, /* Heat level 26 = 18667 Kcal/h */</v>
       </c>
       <c r="S35" s="1"/>
     </row>
@@ -53850,7 +53930,7 @@
         <v>2.3899999999999997</v>
       </c>
       <c r="I36" s="58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="J36" s="58">
@@ -53866,16 +53946,16 @@
         <v>100</v>
       </c>
       <c r="N36" s="56">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>19999.999999999996</v>
       </c>
       <c r="O36" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2.3899999999999997</v>
       </c>
       <c r="Q36" t="str">
-        <f t="shared" si="5"/>
-        <v>{{0, 0, 100}, 20000, 2.39}, /* Heat level 27 = 20000 Kcal/h */</v>
+        <f t="shared" si="7"/>
+        <v>{{0, 0, 100}, 20000, 2,39}, /* Heat level 27 = 20000 Kcal/h */</v>
       </c>
       <c r="S36" s="1"/>
     </row>

</xml_diff>